<commit_message>
Update paypal chrome download dialog missing extension
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Molpaysgdfee/Data/ListReport.xlsx
+++ b/Traveloka_DataAutomation_Portal_Molpaysgdfee/Data/ListReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Portal_Molpaysgdfee\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24A6604-9CEE-4C1A-A7FA-29FA633C07F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDBDD3D-B504-4955-AD00-6E34DD5027A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="1236" windowWidth="17280" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Status</t>
   </si>
@@ -392,7 +392,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A4" sqref="A4:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -489,6 +489,9 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -500,6 +503,9 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -509,6 +515,9 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>